<commit_message>
Updated Sprites and Dialog
# data\chars\Kurt\Talk
    Added frames for talking view
    Removed old placeholder frames
# data\rooms\interactions.xlsx
    Updated script for interaction with the window in the starting room
# unmentioned files
    Added original Polish back into the game for interactions. Need to keep adding more each time I work on this so it's not a big project later on.
    General game asset file changes every time the editor saves.
</commit_message>
<xml_diff>
--- a/data/rooms/interactions.xlsx
+++ b/data/rooms/interactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ciemna Strona\data\rooms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808971E9-C05D-4EFC-BBFA-479A67D1D2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFD2103-4736-4B94-AAA7-C575F9DFD1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6794EB6-DA29-4163-B6D8-200EDABDA398}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6794EB6-DA29-4163-B6D8-200EDABDA398}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Object</t>
   </si>
@@ -52,43 +52,85 @@
     <t>English</t>
   </si>
   <si>
-    <t>this is our kitchen terminal. serving something that pretends to be food so much that it's not edible at all…</t>
-  </si>
-  <si>
-    <t>to nasz terminal kuchenny. serwujĄcy coŚ co tak wysila siĘ udawaniem ŻywnoŚci Że wcale do jedzenia się nie nadaje…</t>
-  </si>
-  <si>
-    <t>Get</t>
-  </si>
-  <si>
-    <t>no, that's a terrible idea.</t>
-  </si>
-  <si>
-    <t>nie, beznadziejny pomysŁ</t>
-  </si>
-  <si>
     <t>Open</t>
   </si>
   <si>
-    <t>to nie możliwe.</t>
-  </si>
-  <si>
-    <t>that's not possible.</t>
-  </si>
-  <si>
     <t>Use</t>
   </si>
   <si>
-    <t>ten terminal używa się, mówiąc do niego. swoją drogą to bardzo wygodne.</t>
-  </si>
-  <si>
-    <t>this terminal is used by speaking to it. It's very convenient, by the way.</t>
-  </si>
-  <si>
     <t>Talk to</t>
   </si>
   <si>
     <t>In Dialog Chat Mapper File</t>
+  </si>
+  <si>
+    <t>The Window</t>
+  </si>
+  <si>
+    <t>"To nie możliwe."</t>
+  </si>
+  <si>
+    <t>"No, that's a terrible idea."</t>
+  </si>
+  <si>
+    <t>"Nie, beznadziejny pomysŁ."</t>
+  </si>
+  <si>
+    <t>"That's not possible."</t>
+  </si>
+  <si>
+    <t>"Ten terminal używa się, mówiąc do niego." "Swoją drogą to bardzo wygodne."</t>
+  </si>
+  <si>
+    <t>"This terminal is used by speaking to it." "It's very convenient, by the way."</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>"Czy wyglądam aż na takiego idiotę?!"</t>
+  </si>
+  <si>
+    <t>"Do I look like an idiot?!"</t>
+  </si>
+  <si>
+    <t>Pick Up</t>
+  </si>
+  <si>
+    <t>"To nasz terminal kuchenny." "SerwujĄcy coŚ co tak wysila siĘ udawaniem ŻywnoŚci Że wcale do jedzenia się nie nadaje..."</t>
+  </si>
+  <si>
+    <t>"This is our kitchen terminal." "Serving something that pretends to be food so much that it's not edible at all..."</t>
+  </si>
+  <si>
+    <t>"Kosmos... Setki Planet... Setki luksusowych hoteli..." "Plaże... Kasyna... Masażystki... I inne atrakcje dostępne dla bogatego wdowca..." "Czyli mnie!"</t>
+  </si>
+  <si>
+    <t>"Space... Hundreds Of Planets... Hundreds of luxury hotels..." "Beaches... Casinos... Masseuses... And other attractions available to a rich widower..." "He... He... He..." "That's me!"</t>
+  </si>
+  <si>
+    <t>"Nie da się..."</t>
+  </si>
+  <si>
+    <t>"I can't..."</t>
+  </si>
+  <si>
+    <t>"Hmmm..." "Dobre..." "Głębokie..." "Hmmm..." "Użyć okna..." "Taaa..." "Aby tak dalej..." "Aby..."</t>
+  </si>
+  <si>
+    <t>"Hmmm..." "Okay..." "Deep..." "Hmmm..." "Use the window..." "Yeah..." "Do keep it up..." "Do..."</t>
+  </si>
+  <si>
+    <t>"Chwileczke.. Zastanów się..."</t>
+  </si>
+  <si>
+    <t>"Wait a minute.. Think about it..."</t>
+  </si>
+  <si>
+    <t>"Huh" "Jest przecież zamknięte!!!"</t>
+  </si>
+  <si>
+    <t>"Huh" "It's closed!!!"</t>
   </si>
 </sst>
 </file>
@@ -112,7 +154,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -120,14 +162,124 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -443,125 +595,591 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A541A8CD-E521-4FA4-BC55-12A663257705}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="107.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="68.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="65" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="135.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="162" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="87.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="88.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="2"/>
       <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="5"/>
+      <c r="L1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="13"/>
+    </row>
+    <row r="2" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="G3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="H3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="B4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="1"/>
+      <c r="E4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="6"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="6"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="6"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="6"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="6"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="6"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="6"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="6"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="6"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="6"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="6"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="6"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="6"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="6"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="6"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="6"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="6"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="6"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="6"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>